<commit_message>
Fix Magasin and facturation
dsqqsdqs
</commit_message>
<xml_diff>
--- a/src/Rapport Magasin.xlsx
+++ b/src/Rapport Magasin.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,22 +499,22 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>55517</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>754190</t>
+          <t>077433</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -524,11 +524,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
@@ -543,22 +543,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>55517</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>118367</t>
+          <t>098899</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -568,7 +568,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -587,22 +587,22 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>55517</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>843091</t>
+          <t>117147</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -612,11 +612,11 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
@@ -631,22 +631,22 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>03692</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>081842</t>
+          <t>116631</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -656,11 +656,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
@@ -675,22 +675,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>03692</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>098830</t>
+          <t>121963</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -700,11 +700,11 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
@@ -719,36 +719,36 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>65888</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>803977</t>
+          <t>102981</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>C27</t>
+          <t>C44</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
@@ -763,22 +763,22 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>70624</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>136825</t>
+          <t>121963</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -788,11 +788,11 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
@@ -807,36 +807,36 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>70624</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>011268</t>
+          <t>098899</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>C45</t>
+          <t>C44</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
@@ -851,36 +851,36 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>70624</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>062765</t>
+          <t>117147</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>C7</t>
+          <t>C44</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
@@ -895,22 +895,22 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>70624</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>098511</t>
+          <t>754190</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -920,7 +920,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -939,17 +939,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>70624</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -964,11 +964,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
@@ -983,22 +983,22 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>70624</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>077995</t>
+          <t>116621</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1008,11 +1008,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
@@ -1027,22 +1027,22 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>70624</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>120956</t>
+          <t>098934</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1052,7 +1052,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1071,22 +1071,22 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>65827</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>098934</t>
+          <t>098899</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1096,11 +1096,11 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
@@ -1115,22 +1115,22 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>65827</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>100304</t>
+          <t>134926</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1140,11 +1140,11 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
@@ -1159,36 +1159,36 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>65827</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>031285</t>
+          <t>117147</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>C40</t>
+          <t>C44</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
@@ -1203,22 +1203,22 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>65827</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>116621</t>
+          <t>116632</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1228,11 +1228,11 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
@@ -1247,36 +1247,36 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>65827</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>122546</t>
+          <t>261578</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>C44</t>
+          <t>C15</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
@@ -1291,22 +1291,22 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>01593</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>123223</t>
+          <t>101565</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1316,11 +1316,11 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
@@ -1335,22 +1335,22 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>01593</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>121963</t>
+          <t>100414</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1360,11 +1360,11 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
@@ -1379,22 +1379,22 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>01593</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>097976</t>
+          <t>098899</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1404,11 +1404,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
@@ -1423,36 +1423,36 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>65822</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>043935</t>
+          <t>261578</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>C44</t>
+          <t>C15</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
@@ -1467,32 +1467,32 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>50138</t>
+          <t>65822</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>MAJSER</t>
+          <t>062765</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>999</t>
+          <t>C7</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -1511,22 +1511,22 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>65822</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>105147</t>
+          <t>134926</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1536,7 +1536,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -1555,22 +1555,22 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>65822</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>120171</t>
+          <t>077433</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1580,11 +1580,11 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
@@ -1599,22 +1599,22 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>65864</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>843091</t>
+          <t>121944</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1624,11 +1624,11 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
@@ -1643,22 +1643,22 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>65864</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>081842</t>
+          <t>098899</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1668,11 +1668,11 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
@@ -1687,22 +1687,22 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>65864</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>098830</t>
+          <t>134926</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1712,11 +1712,11 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
@@ -1731,22 +1731,22 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>65864</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>121963</t>
+          <t>117147</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1756,11 +1756,11 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
@@ -1775,22 +1775,22 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>65864</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>150756</t>
+          <t>011765</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1800,11 +1800,11 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>
@@ -1819,22 +1819,22 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>03162</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>043935</t>
+          <t>101565</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -1844,11 +1844,11 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr"/>
@@ -1863,22 +1863,22 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>03162</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>281185</t>
+          <t>100414</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -1888,11 +1888,11 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
@@ -1907,22 +1907,22 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>03162</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>101565</t>
+          <t>117147</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -1932,11 +1932,11 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr"/>
@@ -1951,22 +1951,22 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>03162</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>100414</t>
+          <t>102981</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -1976,11 +1976,11 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr"/>
@@ -1995,22 +1995,22 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>03162</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>120956</t>
+          <t>098934</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -2020,11 +2020,11 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr"/>
@@ -2039,22 +2039,22 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>65818</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>102981</t>
+          <t>121944</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -2064,11 +2064,11 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
@@ -2083,22 +2083,22 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>65818</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>135793</t>
+          <t>754190</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -2108,7 +2108,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -2127,22 +2127,22 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>65818</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>102158</t>
+          <t>120171</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -2152,11 +2152,11 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
@@ -2171,22 +2171,22 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>65818</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>100304</t>
+          <t>843120</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -2196,11 +2196,11 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr"/>
@@ -2215,22 +2215,22 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>65818</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>122546</t>
+          <t>081842</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -2240,11 +2240,11 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr"/>
@@ -2259,36 +2259,36 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>65818</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>134926</t>
+          <t>803977</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>C44</t>
+          <t>C27</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr"/>
@@ -2303,22 +2303,22 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>65818</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>097675</t>
+          <t>182953</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -2328,11 +2328,11 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
@@ -2347,32 +2347,32 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>729</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>23922</t>
+          <t>65818</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>MAJSER</t>
+          <t>031551</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>999</t>
+          <t>C44</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>290724</t>
+          <t>310724</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -2381,6 +2381,1194 @@
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>44</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>729</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>65818</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>116648</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I45" t="n">
+        <v>5</v>
+      </c>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>45</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>729</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>65818</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>097675</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I46" t="n">
+        <v>5</v>
+      </c>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>46</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>729</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>65818</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>062765</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>C7</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I47" t="n">
+        <v>1</v>
+      </c>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>47</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>729</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>65818</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>122546</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I48" t="n">
+        <v>6</v>
+      </c>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>48</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>729</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>65874</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>121963</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I49" t="n">
+        <v>20</v>
+      </c>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>49</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>729</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>65874</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>098899</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I50" t="n">
+        <v>2</v>
+      </c>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>50</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>729</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>65874</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>134926</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I51" t="n">
+        <v>2</v>
+      </c>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>51</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>729</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>65874</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>043935</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I52" t="n">
+        <v>1</v>
+      </c>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>52</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>65870</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>062765</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>C7</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I53" t="n">
+        <v>1</v>
+      </c>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>53</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>65870</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>134926</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I54" t="n">
+        <v>1</v>
+      </c>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>54</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>65870</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>117147</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I55" t="n">
+        <v>2</v>
+      </c>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>55</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>65870</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>754190</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I56" t="n">
+        <v>2</v>
+      </c>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>56</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>65870</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>043935</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I57" t="n">
+        <v>1</v>
+      </c>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>57</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>65805</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>117147</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I58" t="n">
+        <v>4</v>
+      </c>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>58</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>65805</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>098934</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I59" t="n">
+        <v>2</v>
+      </c>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>59</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>65805</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>098899</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I60" t="n">
+        <v>2</v>
+      </c>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
+      <c r="L60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>60</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>65805</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>116648</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I61" t="n">
+        <v>10</v>
+      </c>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr"/>
+      <c r="L61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>61</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>65805</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>122546</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I62" t="n">
+        <v>50</v>
+      </c>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr"/>
+      <c r="L62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>62</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>65870</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>011765</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I63" t="n">
+        <v>30</v>
+      </c>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr"/>
+      <c r="L63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>63</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>65843</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>136825</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I64" t="n">
+        <v>4</v>
+      </c>
+      <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr"/>
+      <c r="L64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>64</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>65843</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>098934</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I65" t="n">
+        <v>2</v>
+      </c>
+      <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
+      <c r="L65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>65</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>65843</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>116621</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I66" t="n">
+        <v>2</v>
+      </c>
+      <c r="J66" t="inlineStr"/>
+      <c r="K66" t="inlineStr"/>
+      <c r="L66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>66</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>65877</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>134926</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I67" t="n">
+        <v>1</v>
+      </c>
+      <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr"/>
+      <c r="L67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>67</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>65877</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>098899</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I68" t="n">
+        <v>8</v>
+      </c>
+      <c r="J68" t="inlineStr"/>
+      <c r="K68" t="inlineStr"/>
+      <c r="L68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>68</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>65877</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>105147</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I69" t="n">
+        <v>15</v>
+      </c>
+      <c r="J69" t="inlineStr"/>
+      <c r="K69" t="inlineStr"/>
+      <c r="L69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>69</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>65877</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>754190</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I70" t="n">
+        <v>2</v>
+      </c>
+      <c r="J70" t="inlineStr"/>
+      <c r="K70" t="inlineStr"/>
+      <c r="L70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>70</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>65877</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>121944</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>C44</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>310724</t>
+        </is>
+      </c>
+      <c r="I71" t="n">
+        <v>30</v>
+      </c>
+      <c r="J71" t="inlineStr"/>
+      <c r="K71" t="inlineStr"/>
+      <c r="L71" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>